<commit_message>
Fix CCDI locators, add TC01 for phs002517, add TSV/UI normalization, and data hub fixes
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing.xlsx
+++ b/InputFiles/CCDI/TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0417\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF2B03E-C417-410F-B6B8-F821452FDD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFB4CC-A961-F241-A0EA-E1A2052BE22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="4560" yWindow="-27960" windowWidth="35960" windowHeight="24600" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,161 +112,280 @@
 left join funding f on s.study_id = f.study </t>
   </si>
   <si>
+    <t>TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing_TSVData.xlsx</t>
+  </si>
+  <si>
     <t>WITH filtered_seq AS (
-    SELECT *
-    FROM df_sequencing_file
-    WHERE file_type = 'bai'
-      AND library_selection = 'Hybrid Selection'
-      AND library_strategy = 'WXS'
-      AND data_category = 'Sequencing'
+  SELECT *
+  FROM df_sequencing_file
+  WHERE file_type = 'bai'
+    AND library_selection = 'Hybrid Selection'
+    AND library_strategy = 'WXS'
+    AND data_category = 'Sequencing'
 )
 SELECT
-    COUNT(DISTINCT s.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT seq.sequencing_file_id) AS "Sequencing Files"
-FROM filtered_seq seq
-JOIN df_sample smp ON seq."sample.id" = smp.id
-JOIN df_participant p ON smp."participant.id" = p.id
-JOIN df_study s ON p."study.id" = s.id
-WHERE s.dbgap_accession = 'phs002517';</t>
-  </si>
-  <si>
-    <t>WITH diagnosis_summary AS ( 
-    SELECT 
-        dgn."participant.id" AS participant_id, 
-        GROUP_CONCAT(DISTINCT dgn.age_at_diagnosis) AS age_at_diagnosis, 
-        GROUP_CONCAT(DISTINCT dgn.diagnosis) AS diagnosis, 
-        GROUP_CONCAT(DISTINCT dgn.anatomic_site) AS anatomic_site,
-        GROUP_CONCAT(DISTINCT dgn.diagnosis_basis) AS diagnosis_basis
-    FROM df_diagnosis dgn
-    WHERE dgn."participant.id" IS NOT NULL
-    GROUP BY dgn."participant.id"
+  COUNT(DISTINCT std.dbgap_accession) AS "Studies",
+  COUNT(DISTINCT prt.participant_id)  AS "Participants",
+  COUNT(DISTINCT smp.sample_id)       AS "Samples",
+  COUNT(DISTINCT seq.id)              AS "Sequencing Files"
+FROM df_study std
+JOIN df_consent_group cg
+  ON cg."study.id" = std.id
+JOIN df_participant prt
+  ON prt."consent_group.id" = cg.id
+JOIN df_sample smp
+  ON smp."participant.id" = prt.id
+JOIN filtered_seq seq
+  ON seq."sample.id" = smp.id
+WHERE std.dbgap_accession = 'phs002517';</t>
+  </si>
+  <si>
+    <t>WITH filtered_seq AS (
+  SELECT *
+  FROM df_sequencing_file
+  WHERE file_type = 'bai'
+    AND library_selection = 'Hybrid Selection'
+    AND library_strategy  = 'WXS'
+    AND data_category     = 'Sequencing'
 ),
-survival_summary AS (
-    SELECT 
-        "participant.id" AS participant_id,
-        GROUP_CONCAT(DISTINCT last_known_survival_status) AS last_known_survival_status
-    FROM df_survival
-    WHERE last_known_survival_status IS NOT NULL
-    GROUP BY "participant.id"
+base AS (
+  SELECT 
+      prt.id              AS participant_pk,
+      prt.participant_id,
+      prt.sex_at_birth,
+      prt.race,
+      std.dbgap_accession
+  FROM df_study std
+  JOIN df_consent_group cg 
+    ON cg."study.id" = std.id
+  JOIN df_participant prt  
+    ON prt."consent_group.id" = cg.id
+  WHERE std.dbgap_accession = 'phs002517'
+    AND EXISTS (
+      SELECT 1
+      FROM df_sample smp
+      JOIN filtered_seq f ON f."sample.id" = smp.id
+      WHERE smp."participant.id" = prt.id
+    )
 )
 SELECT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-    COALESCE(dgn.diagnosis, '') AS "Diagnosis",
-    COALESCE(dgn.anatomic_site, '') AS "Diagnosis Anatomic Site",
-    COALESCE(
+  b.participant_id                                    AS "Participant ID",
+  b.dbgap_accession                                   AS "Study ID",
+  COALESCE(b.sex_at_birth, '')                        AS "Sex",
+  COALESCE(b.race, '')                                AS "Race",
+  /* Diagnosis (stable alphabetical) */
+  COALESCE((
+    SELECT GROUP_CONCAT(val, ';')
+    FROM (
+      SELECT DISTINCT TRIM(dgn.diagnosis) AS val
+      FROM df_diagnosis dgn
+      WHERE dgn."participant.id" = b.participant_pk
+        AND dgn.diagnosis IS NOT NULL
+        AND dgn.diagnosis &lt;&gt; ''
+      ORDER BY LOWER(val)
+    )
+  ), '')                                              AS "Diagnosis",
+  /* Anatomic Site (stable alphabetical) */
+  COALESCE((
+    SELECT GROUP_CONCAT(val, ';')
+    FROM (
+      SELECT DISTINCT TRIM(dgn.anatomic_site) AS val
+      FROM df_diagnosis dgn
+      WHERE dgn."participant.id" = b.participant_pk
+        AND dgn.anatomic_site IS NOT NULL
+        AND dgn.anatomic_site &lt;&gt; ''
+      ORDER BY LOWER(val)
+    )
+  ), '')                                              AS "Diagnosis Anatomic Site",
+  /* Diagnosis Category (stable alphabetical) */
+  COALESCE((
+    SELECT GROUP_CONCAT(val, ';')
+    FROM (
+      SELECT DISTINCT TRIM(dgn.diagnosis_category) AS val
+      FROM df_diagnosis dgn
+      WHERE dgn."participant.id" = b.participant_pk
+        AND dgn.diagnosis_category IS NOT NULL
+        AND dgn.diagnosis_category &lt;&gt; ''
+      ORDER BY LOWER(val)
+    )
+  ), '')                                              AS "Diagnosis Category",
+  /* Age at Diagnosis (replace -999, stable numeric-string order) */
+  COALESCE((
+    SELECT GROUP_CONCAT(val, ';')
+    FROM (
+      SELECT DISTINCT
         CASE 
-            WHEN dgn.age_at_diagnosis = '-999' THEN 'Not Reported'
-            ELSE dgn.age_at_diagnosis 
-        END, ''
-    ) AS "Age at Diagnosis (days)",
-    null AS "Treatment Type",
-    COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
-FROM df_participant prt
-JOIN df_study std ON prt."study.id" = std.id
-LEFT JOIN diagnosis_summary dgn ON prt.id = dgn.participant_id
-LEFT JOIN survival_summary srv ON prt.id = srv.participant_id
-WHERE std.dbgap_accession = 'phs002517'
-  AND EXISTS (
-      SELECT 1 
-      FROM df_sample smp
-      JOIN df_sequencing_file f ON f."sample.id" = smp.id
-      WHERE smp."participant.id" = prt.id
-        AND f.file_type = 'bai'
-        AND f.library_selection = 'Hybrid Selection'
-        AND f.library_strategy = 'WXS'
-        AND f.data_category = 'Sequencing'
-  )
-ORDER BY prt.participant_id ASC
-Limit 100 ;</t>
-  </si>
-  <si>
-    <t>WITH filtered_sequencing_files AS (
-    SELECT 
-        f.file_name, 
-        f.data_category, 
-        f.file_type, 
-        f.file_description, 
-        f.file_size, 
-        f.file_access,
-        smp.sample_id AS actual_sample_id, 
-        prt.participant_id AS actual_participant_id,
-        std.dbgap_accession
-    FROM df_sequencing_file f
-    JOIN df_sample smp ON f."sample.id" = smp.id
-    JOIN df_participant prt ON smp."participant.id" = prt.id
-    JOIN df_study std ON prt."study.id" = std.id
-    WHERE f.file_type = 'bai'
-      AND f.library_selection = 'Hybrid Selection'
-      AND f.library_strategy = 'WXS'
-      AND f.data_category = 'Sequencing'
-      AND std.dbgap_accession = 'phs002517'
+          WHEN TRIM(dgn.age_at_diagnosis) = '-999' THEN 'Not Reported'
+          ELSE TRIM(dgn.age_at_diagnosis)
+        END AS val
+      FROM df_diagnosis dgn
+      WHERE dgn."participant.id" = b.participant_pk
+        AND dgn.age_at_diagnosis IS NOT NULL
+        AND dgn.age_at_diagnosis &lt;&gt; ''
+      ORDER BY val
+    )
+  ), '')                                              AS "Age at Diagnosis (days)",
+  NULL                                                AS "Treatment Type",
+  /* Last Known Survival Status (stable alphabetical) */
+  COALESCE((
+    SELECT GROUP_CONCAT(val, ';')
+    FROM (
+      SELECT DISTINCT TRIM(sv.last_known_survival_status) AS val
+      FROM df_survival sv
+      WHERE sv."participant.id" = b.participant_pk
+        AND sv.last_known_survival_status IS NOT NULL
+        AND sv.last_known_survival_status &lt;&gt; ''
+      ORDER BY LOWER(val)
+    )
+  ), '')                                              AS "Last Known Survival Status"
+FROM base b
+ORDER BY b.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH filtered_seq AS (
+  SELECT 
+    f.file_name,
+    COALESCE(f.data_category, 'Sequencing')      AS data_category,
+    COALESCE(f.file_description, '')             AS file_description,
+    COALESCE(f.file_type, '')                    AS file_type,
+    /* cast in case file_size is text; keep raw value for formatting */
+    CAST(f.file_size AS REAL)                    AS file_size_num,
+    COALESCE(f.file_access, '')                  AS file_access,
+    smp.sample_id                                AS "Sample ID",
+    prt.participant_id                           AS "Participant ID",
+    std.dbgap_accession                          AS "Study ID"
+  FROM df_sequencing_file f
+  JOIN df_sample smp
+    ON smp.id = f."sample.id"
+  JOIN df_participant prt
+    ON prt.id = smp."participant.id"
+  JOIN df_consent_group cg
+    ON cg.id = prt."consent_group.id"
+  JOIN df_study std
+    ON std.id = cg."study.id"
+  WHERE f.file_type         = 'bai'
+    AND f.library_selection = 'Hybrid Selection'
+    AND f.library_strategy  = 'WXS'
+    AND f.data_category     = 'Sequencing'
+    AND std.dbgap_accession = 'phs002517'
 )
 SELECT DISTINCT
-    f.file_name AS "File Name",
-    f.data_category AS "Data Category",
-    COALESCE(f.file_description, '') AS "File Description",
-    f.file_type AS "File Type",
-    CASE
-        WHEN f.file_size &gt;= 1024 * 1024 * 1024 THEN ROUND(f.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        WHEN f.file_size &gt;= 1024 * 1024 THEN ROUND(f.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        WHEN f.file_size &gt;= 1024 THEN ROUND(f.file_size / 1024.0, 2) || ' KB'
-        ELSE ROUND(f.file_size, 2) || ' Bytes'
-    END AS "File Size",
-    f.file_access AS "File Access",
-    f.dbgap_accession AS "Study ID",
-    f.actual_participant_id AS "Participant ID",
-    f.actual_sample_id AS "Sample ID"
-FROM filtered_sequencing_files f
-ORDER BY f.file_name
-Limit 100 ;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT   
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    COALESCE(
-        CASE 
-            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' 
-            ELSE smp.participant_age_at_collection 
-        END, 
-        0
-    ) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    CASE 
-        WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis
-        ELSE ''
-    END AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN df_participant prt ON std.id = prt."study.id"
-LEFT JOIN df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN df_diagnosis dgn ON smp.id = dgn."sample.id"
-LEFT JOIN df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN df_sequencing_file f ON smp.id = f."sample.id"
-WHERE 
-    f.file_type = 'bai'
-    AND f.library_selection = 'Hybrid Selection'
-    AND f.library_strategy = 'WXS'
-    AND f.data_category = 'Sequencing'
-    AND std.dbgap_accession = 'phs002517'
-    AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC
-Limit 100 ;</t>
-  </si>
-  <si>
-    <t>TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>TC02_CCDI_phs002517_FileType-bai_LibStr-WXS_LibSel-HybSel_DC-Sequencing_TSVData.xlsx</t>
+  file_name                                   AS "File Name",
+  data_category                                AS "Data Category",
+  file_description                             AS "File Description",
+  file_type                                    AS "File Type",
+  CASE
+    WHEN file_size_num IS NULL                     THEN ''
+    WHEN file_size_num &gt;= 1024*1024*1024           THEN ROUND(file_size_num / (1024.0*1024.0*1024.0), 2) || ' GB'
+    WHEN file_size_num &gt;= 1024*1024                THEN ROUND(file_size_num / (1024.0*1024.0), 2) || ' MB'
+    WHEN file_size_num &gt;= 1024                     THEN ROUND(file_size_num / 1024.0, 2) || ' KB'
+    ELSE ROUND(file_size_num, 2) || ' Bytes'
+  END                                           AS "File Size",
+  file_access                                   AS "File Access",
+  "Study ID"                                     AS "Study ID",
+  "Participant ID"                               AS "Participant ID",
+  "Sample ID"                                    AS "Sample ID"
+FROM filtered_seq
+ORDER BY "File Name" ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH filtered_seq AS (
+  /* Samples that have the specific sequencing files */
+  SELECT DISTINCT "sample.id"
+  FROM df_sequencing_file
+  WHERE file_type         = 'bai'
+    AND library_selection = 'Hybrid Selection'
+    AND library_strategy  = 'WXS'
+    AND data_category     = 'Sequencing'
+),
+/* Keep only diagnosis rows that look like the UI’s “primary/pathology” signal.
+   - Basis: histologic / pathology (common spellings)
+   - Category: exclude benign/normal/non-cancer
+*/
+allowed_dx AS (
+  SELECT
+    d."sample.id"              AS sample_fk,
+    TRIM(d.diagnosis)          AS diagnosis,
+    TRIM(d.diagnosis_category) AS diagnosis_category
+  FROM df_diagnosis d
+  WHERE d."sample.id" IS NOT NULL
+    AND d.diagnosis IS NOT NULL
+    AND TRIM(d.diagnosis) &lt;&gt; ''
+    AND (
+      /* Pathology / histology-only basis (allow NULL to avoid over-pruning if UI does too) */
+      LOWER(COALESCE(d.diagnosis_basis,'')) IN ('histologic','pathologic','pathology','microscopic')
+      OR d.diagnosis_basis IS NULL
+    )
+    AND LOWER(COALESCE(d.diagnosis_category,'')) NOT IN ('normal','non-cancer','noncancer','benign')
+),
+dx_by_sample AS (
+  /* DISTINCT + GROUP_CONCAT with a separator (SQLite needs DISTINCT to have one argument)
+     so we distinct the rows first, then concat */
+  SELECT
+    sample_fk,
+    GROUP_CONCAT(diagnosis, '; ') AS diagnosis
+  FROM (
+    SELECT DISTINCT sample_fk, diagnosis
+    FROM allowed_dx
+    WHERE diagnosis IS NOT NULL AND diagnosis &lt;&gt; ''
+  ) x
+  GROUP BY sample_fk
+),
+dxcat_by_sample AS (
+  SELECT
+    sample_fk,
+    GROUP_CONCAT(diagnosis_category, '; ') AS diagnosis_category
+  FROM (
+    SELECT DISTINCT sample_fk, diagnosis_category
+    FROM allowed_dx
+    WHERE diagnosis_category IS NOT NULL AND diagnosis_category &lt;&gt; ''
+  ) y
+  GROUP BY sample_fk
+)
+SELECT DISTINCT
+  smp.sample_id                         AS "Sample ID",
+  prt.participant_id                    AS "Participant ID",
+  std.dbgap_accession                   AS "Study ID",
+  COALESCE(smp.anatomic_site, '')       AS "Sample Anatomic Site",
+  CASE
+    WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported'
+    WHEN smp.participant_age_at_collection IS NULL THEN ''
+    ELSE CAST(smp.participant_age_at_collection AS TEXT)
+  END                                    AS "Age at Sample Collection (days)",
+  COALESCE(smp.sample_tumor_status, '')  AS "Sample Tumor Status",
+  COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
+  /* Suppress diagnosis for clearly non-tumor samples */
+  CASE
+    WHEN LOWER(COALESCE(smp.sample_tumor_status, '')) IN ('normal','non-cancer','noncancer','benign')
+      OR LOWER(COALESCE(smp.tumor_classification, '')) IN ('normal','non-cancer','noncancer','benign')
+      THEN ''
+    ELSE COALESCE(dx.diagnosis, '')
+  END                                    AS "Sample Diagnosis",
+  CASE
+    WHEN LOWER(COALESCE(smp.sample_tumor_status, '')) IN ('normal','non-cancer','noncancer','benign')
+      OR LOWER(COALESCE(smp.tumor_classification, '')) IN ('normal','non-cancer','noncancer','benign')
+      THEN ''
+    ELSE COALESCE(dxcat.diagnosis_category, '')
+  END                                    AS "Diagnosis Category"
+FROM df_study std
+JOIN df_consent_group cg
+  ON cg."study.id" = std.id
+JOIN df_participant prt
+  ON prt."consent_group.id" = cg.id
+JOIN df_sample smp
+  ON smp."participant.id" = prt.id
+LEFT JOIN dx_by_sample     dx    ON dx.sample_fk    = smp.id
+LEFT JOIN dxcat_by_sample  dxcat ON dxcat.sample_fk = smp.id
+WHERE std.dbgap_accession = 'phs002517'
+  AND EXISTS (SELECT 1 FROM filtered_seq fs WHERE fs."sample.id" = smp.id)
+  AND smp.sample_id IS NOT NULL
+ORDER BY smp.sample_id ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -668,19 +787,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="90.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -697,24 +816,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -723,29 +842,29 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>